<commit_message>
Update Marathon Training Plan.xlsx
</commit_message>
<xml_diff>
--- a/Marathon Training Plan.xlsx
+++ b/Marathon Training Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Github\Sports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FFE6B4D-FD03-42F1-B100-0833FB102285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7933FA4-A710-431B-B27B-4BB638AB7EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{1961EE94-FA69-4DAC-8A9A-5877D820473B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{1961EE94-FA69-4DAC-8A9A-5877D820473B}"/>
   </bookViews>
   <sheets>
     <sheet name="S+C" sheetId="1" r:id="rId1"/>
@@ -301,7 +301,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -317,6 +317,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -349,16 +355,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -372,6 +375,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -920,7 +929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED425E8E-3BB1-445A-B436-2D42CD55E47C}">
   <dimension ref="B26"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -944,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5B4D158-2BF8-4ECA-B6FD-64FBC00CF41D}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -956,7 +965,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="119.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>75</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -982,28 +991,28 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="119.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="5" t="s">
+      <c r="F2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1011,25 +1020,25 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="F3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1037,25 +1046,25 @@
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="6" t="s">
+      <c r="F4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1063,25 +1072,25 @@
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="6" t="s">
+      <c r="F5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1089,25 +1098,25 @@
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="6" t="s">
+      <c r="F6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1115,25 +1124,25 @@
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="6" t="s">
+      <c r="F7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="4" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1141,25 +1150,25 @@
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="6" t="s">
+      <c r="F8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="4" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1167,25 +1176,25 @@
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="6" t="s">
+      <c r="F9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="4" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1193,25 +1202,25 @@
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="7" t="s">
+      <c r="B10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="6" t="s">
+      <c r="F10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="4" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1219,25 +1228,25 @@
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="6" t="s">
+      <c r="F11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1245,25 +1254,25 @@
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="B12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="6" t="s">
+      <c r="F12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1271,25 +1280,25 @@
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="B13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="6" t="s">
+      <c r="F13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="4" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1297,25 +1306,25 @@
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="B14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="6" t="s">
+      <c r="F14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="4" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1323,25 +1332,25 @@
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="7" t="s">
+      <c r="B15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="6" t="s">
+      <c r="F15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="4" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1349,25 +1358,25 @@
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="6" t="s">
+      <c r="B16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="6" t="s">
+      <c r="F16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1375,25 +1384,25 @@
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="B17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="6" t="s">
+      <c r="E17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="5" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>